<commit_message>
conduct tests for S1 Graphql 2000 users
</commit_message>
<xml_diff>
--- a/Wyniki 3/Gotowe!/S4s.xlsx
+++ b/Wyniki 3/Gotowe!/S4s.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kacpe\OneDrive\Pulpit\Projekty\Praca magisterska\Wyniki 3\Gotowe!\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83B762E6-03FE-46BA-9AA8-79F6AF95D9AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB757572-D8CC-4C2B-821E-63A41D06E35A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -553,17 +553,17 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -849,8 +849,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="G3:O28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C3" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -861,17 +861,17 @@
   </cols>
   <sheetData>
     <row r="3" spans="7:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
     </row>
     <row r="4" spans="7:15" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G4" s="5" t="s">
@@ -903,7 +903,7 @@
       </c>
     </row>
     <row r="5" spans="7:15" x14ac:dyDescent="0.25">
-      <c r="G5" s="7">
+      <c r="G5" s="8">
         <v>100</v>
       </c>
       <c r="H5" s="4" t="s">
@@ -921,18 +921,18 @@
       <c r="L5" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="M5" s="8" t="s">
+      <c r="M5" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="N5" s="8" t="s">
+      <c r="N5" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="O5" s="8" t="s">
+      <c r="O5" s="6" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="6" spans="7:15" x14ac:dyDescent="0.25">
-      <c r="G6" s="7"/>
+      <c r="G6" s="8"/>
       <c r="H6" s="4" t="s">
         <v>12</v>
       </c>
@@ -948,18 +948,18 @@
       <c r="L6" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="M6" s="8" t="s">
+      <c r="M6" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="N6" s="8" t="s">
+      <c r="N6" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="O6" s="8" t="s">
+      <c r="O6" s="6" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="7" spans="7:15" x14ac:dyDescent="0.25">
-      <c r="G7" s="7"/>
+      <c r="G7" s="8"/>
       <c r="H7" s="4" t="s">
         <v>13</v>
       </c>
@@ -975,18 +975,18 @@
       <c r="L7" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="M7" s="8" t="s">
+      <c r="M7" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="N7" s="8" t="s">
+      <c r="N7" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="O7" s="8" t="s">
+      <c r="O7" s="6" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="8" spans="7:15" x14ac:dyDescent="0.25">
-      <c r="G8" s="7"/>
+      <c r="G8" s="8"/>
       <c r="H8" s="4" t="s">
         <v>14</v>
       </c>
@@ -1002,18 +1002,18 @@
       <c r="L8" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="M8" s="8" t="s">
+      <c r="M8" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="N8" s="8" t="s">
+      <c r="N8" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="O8" s="8" t="s">
+      <c r="O8" s="6" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="9" spans="7:15" x14ac:dyDescent="0.25">
-      <c r="G9" s="7"/>
+      <c r="G9" s="8"/>
       <c r="H9" s="4" t="s">
         <v>7</v>
       </c>
@@ -1029,18 +1029,18 @@
       <c r="L9" s="1">
         <v>83795</v>
       </c>
-      <c r="M9" s="8">
+      <c r="M9" s="6">
         <v>83796.600000000006</v>
       </c>
-      <c r="N9" s="8">
+      <c r="N9" s="6">
         <v>83791.399999999994</v>
       </c>
-      <c r="O9" s="8">
+      <c r="O9" s="6">
         <v>83852.399999999994</v>
       </c>
     </row>
     <row r="10" spans="7:15" x14ac:dyDescent="0.25">
-      <c r="G10" s="7"/>
+      <c r="G10" s="8"/>
       <c r="H10" s="4" t="s">
         <v>8</v>
       </c>
@@ -1056,18 +1056,18 @@
       <c r="L10" s="1">
         <v>87.23</v>
       </c>
-      <c r="M10" s="8">
+      <c r="M10" s="6">
         <v>87.23</v>
       </c>
-      <c r="N10" s="8">
+      <c r="N10" s="6">
         <v>87.22</v>
       </c>
-      <c r="O10" s="8">
+      <c r="O10" s="6">
         <v>87.28</v>
       </c>
     </row>
     <row r="11" spans="7:15" x14ac:dyDescent="0.25">
-      <c r="G11" s="7"/>
+      <c r="G11" s="8"/>
       <c r="H11" s="4" t="s">
         <v>9</v>
       </c>
@@ -1083,18 +1083,18 @@
       <c r="L11" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="M11" s="8" t="s">
+      <c r="M11" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="N11" s="8" t="s">
+      <c r="N11" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="O11" s="8" t="s">
+      <c r="O11" s="6" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="12" spans="7:15" x14ac:dyDescent="0.25">
-      <c r="G12" s="7"/>
+      <c r="G12" s="8"/>
       <c r="H12" s="4" t="s">
         <v>10</v>
       </c>
@@ -1110,18 +1110,18 @@
       <c r="L12" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="M12" s="8" t="s">
+      <c r="M12" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="N12" s="8" t="s">
+      <c r="N12" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="O12" s="8" t="s">
+      <c r="O12" s="6" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="13" spans="7:15" x14ac:dyDescent="0.25">
-      <c r="G13" s="7">
+      <c r="G13" s="8">
         <v>1000</v>
       </c>
       <c r="H13" s="4" t="s">
@@ -1139,18 +1139,18 @@
       <c r="L13" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="M13" s="9" t="s">
+      <c r="M13" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="N13" s="9" t="s">
+      <c r="N13" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="O13" s="9" t="s">
+      <c r="O13" s="7" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="14" spans="7:15" x14ac:dyDescent="0.25">
-      <c r="G14" s="7"/>
+      <c r="G14" s="8"/>
       <c r="H14" s="4" t="s">
         <v>12</v>
       </c>
@@ -1166,18 +1166,18 @@
       <c r="L14" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="M14" s="9" t="s">
+      <c r="M14" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="N14" s="9" t="s">
+      <c r="N14" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="O14" s="9" t="s">
+      <c r="O14" s="7" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="15" spans="7:15" x14ac:dyDescent="0.25">
-      <c r="G15" s="7"/>
+      <c r="G15" s="8"/>
       <c r="H15" s="4" t="s">
         <v>13</v>
       </c>
@@ -1193,18 +1193,18 @@
       <c r="L15" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="M15" s="9" t="s">
+      <c r="M15" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="N15" s="9" t="s">
+      <c r="N15" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="O15" s="9" t="s">
+      <c r="O15" s="7" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="16" spans="7:15" x14ac:dyDescent="0.25">
-      <c r="G16" s="7"/>
+      <c r="G16" s="8"/>
       <c r="H16" s="4" t="s">
         <v>14</v>
       </c>
@@ -1220,18 +1220,18 @@
       <c r="L16" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="M16" s="9" t="s">
+      <c r="M16" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="N16" s="9" t="s">
+      <c r="N16" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="O16" s="9" t="s">
+      <c r="O16" s="7" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="17" spans="7:15" x14ac:dyDescent="0.25">
-      <c r="G17" s="7"/>
+      <c r="G17" s="8"/>
       <c r="H17" s="4" t="s">
         <v>7</v>
       </c>
@@ -1247,18 +1247,18 @@
       <c r="L17" s="2">
         <v>837463</v>
       </c>
-      <c r="M17" s="9">
+      <c r="M17" s="7">
         <v>837949</v>
       </c>
-      <c r="N17" s="9">
+      <c r="N17" s="7">
         <v>838073</v>
       </c>
-      <c r="O17" s="9">
+      <c r="O17" s="7">
         <v>839066</v>
       </c>
     </row>
     <row r="18" spans="7:15" x14ac:dyDescent="0.25">
-      <c r="G18" s="7"/>
+      <c r="G18" s="8"/>
       <c r="H18" s="4" t="s">
         <v>8</v>
       </c>
@@ -1274,18 +1274,18 @@
       <c r="L18" s="2">
         <v>873.03</v>
       </c>
-      <c r="M18" s="9">
+      <c r="M18" s="7">
         <v>872.12</v>
       </c>
-      <c r="N18" s="9">
+      <c r="N18" s="7">
         <v>872.3</v>
       </c>
-      <c r="O18" s="9">
+      <c r="O18" s="7">
         <v>873.3</v>
       </c>
     </row>
     <row r="19" spans="7:15" x14ac:dyDescent="0.25">
-      <c r="G19" s="7"/>
+      <c r="G19" s="8"/>
       <c r="H19" s="4" t="s">
         <v>9</v>
       </c>
@@ -1301,18 +1301,18 @@
       <c r="L19" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="M19" s="9" t="s">
+      <c r="M19" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="N19" s="9" t="s">
+      <c r="N19" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="O19" s="9" t="s">
+      <c r="O19" s="7" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="20" spans="7:15" x14ac:dyDescent="0.25">
-      <c r="G20" s="7"/>
+      <c r="G20" s="8"/>
       <c r="H20" s="4" t="s">
         <v>10</v>
       </c>
@@ -1328,18 +1328,18 @@
       <c r="L20" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="M20" s="9" t="s">
+      <c r="M20" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="N20" s="9" t="s">
+      <c r="N20" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="O20" s="9" t="s">
+      <c r="O20" s="7" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="21" spans="7:15" x14ac:dyDescent="0.25">
-      <c r="G21" s="7">
+      <c r="G21" s="8">
         <v>4000</v>
       </c>
       <c r="H21" s="4" t="s">
@@ -1357,18 +1357,18 @@
       <c r="L21" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="M21" s="8" t="s">
+      <c r="M21" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="N21" s="8" t="s">
+      <c r="N21" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="O21" s="8" t="s">
+      <c r="O21" s="6" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="22" spans="7:15" x14ac:dyDescent="0.25">
-      <c r="G22" s="7"/>
+      <c r="G22" s="8"/>
       <c r="H22" s="4" t="s">
         <v>12</v>
       </c>
@@ -1384,18 +1384,18 @@
       <c r="L22" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="M22" s="8" t="s">
+      <c r="M22" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="N22" s="8" t="s">
+      <c r="N22" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="O22" s="8" t="s">
+      <c r="O22" s="6" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="23" spans="7:15" x14ac:dyDescent="0.25">
-      <c r="G23" s="7"/>
+      <c r="G23" s="8"/>
       <c r="H23" s="4" t="s">
         <v>13</v>
       </c>
@@ -1411,18 +1411,18 @@
       <c r="L23" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="M23" s="8" t="s">
+      <c r="M23" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="N23" s="8" t="s">
+      <c r="N23" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="O23" s="8" t="s">
+      <c r="O23" s="6" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="24" spans="7:15" x14ac:dyDescent="0.25">
-      <c r="G24" s="7"/>
+      <c r="G24" s="8"/>
       <c r="H24" s="4" t="s">
         <v>14</v>
       </c>
@@ -1438,18 +1438,18 @@
       <c r="L24" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="M24" s="8" t="s">
+      <c r="M24" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="N24" s="8" t="s">
+      <c r="N24" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="O24" s="8" t="s">
+      <c r="O24" s="6" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="25" spans="7:15" x14ac:dyDescent="0.25">
-      <c r="G25" s="7"/>
+      <c r="G25" s="8"/>
       <c r="H25" s="4" t="s">
         <v>7</v>
       </c>
@@ -1465,18 +1465,18 @@
       <c r="L25" s="1">
         <v>1037282</v>
       </c>
-      <c r="M25" s="8">
+      <c r="M25" s="6">
         <v>1018262</v>
       </c>
-      <c r="N25" s="8">
+      <c r="N25" s="6">
         <v>1101998</v>
       </c>
-      <c r="O25" s="8">
+      <c r="O25" s="6">
         <v>1410614</v>
       </c>
     </row>
     <row r="26" spans="7:15" x14ac:dyDescent="0.25">
-      <c r="G26" s="7"/>
+      <c r="G26" s="8"/>
       <c r="H26" s="4" t="s">
         <v>8</v>
       </c>
@@ -1492,18 +1492,18 @@
       <c r="L26" s="1">
         <v>1079.6199999999999</v>
       </c>
-      <c r="M26" s="8">
+      <c r="M26" s="6">
         <v>1059.44</v>
       </c>
-      <c r="N26" s="8">
+      <c r="N26" s="6">
         <v>1147.2</v>
       </c>
-      <c r="O26" s="8">
+      <c r="O26" s="6">
         <v>1468.23</v>
       </c>
     </row>
     <row r="27" spans="7:15" x14ac:dyDescent="0.25">
-      <c r="G27" s="7"/>
+      <c r="G27" s="8"/>
       <c r="H27" s="4" t="s">
         <v>9</v>
       </c>
@@ -1519,18 +1519,18 @@
       <c r="L27" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="M27" s="8" t="s">
+      <c r="M27" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="N27" s="8" t="s">
+      <c r="N27" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="O27" s="8" t="s">
+      <c r="O27" s="6" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="28" spans="7:15" x14ac:dyDescent="0.25">
-      <c r="G28" s="7"/>
+      <c r="G28" s="8"/>
       <c r="H28" s="4" t="s">
         <v>10</v>
       </c>
@@ -1546,13 +1546,13 @@
       <c r="L28" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="M28" s="8" t="s">
+      <c r="M28" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="N28" s="8" t="s">
+      <c r="N28" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="O28" s="8" t="s">
+      <c r="O28" s="6" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>